<commit_message>
First commit new branch
</commit_message>
<xml_diff>
--- a/Documentation/Lists/Balancing State Locations List.xlsx
+++ b/Documentation/Lists/Balancing State Locations List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/Returns Taxpayer documentation/Lists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{D03E98AE-FEDD-4C8F-96F0-36C099982A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9FE3371-DD24-4DD9-9F9D-C5FC097049A9}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{D03E98AE-FEDD-4C8F-96F0-36C099982A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9451FA0A-31A4-4813-B3EA-E27BC01D32D7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{CCEB6A6A-7B34-4562-B81A-A16DD9604AAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{CCEB6A6A-7B34-4562-B81A-A16DD9604AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="TN" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>TN Checkbox Locatiion</t>
   </si>
@@ -195,6 +195,36 @@
   </si>
   <si>
     <t>Three values needs to be equal to 0</t>
+  </si>
+  <si>
+    <t>State Totals &gt;= County Totals</t>
+  </si>
+  <si>
+    <t>1. Check FilingType = Electronic</t>
+  </si>
+  <si>
+    <t>2. Go to Pre-Creation Check - Check if it has no errors</t>
+  </si>
+  <si>
+    <t>1. Go to Balance page - Ir a columna Balanced Difference - Check if the 3 row values are equals to 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Go to Form CA CDTFA-401 A - Go to page 1 - Get value line 12 </t>
+  </si>
+  <si>
+    <t>3. Go to Form CA CDTFA 531 - Page 1 - Get value in row B5.</t>
+  </si>
+  <si>
+    <t>4. Compare value step 2 vs  value step 3.</t>
+  </si>
+  <si>
+    <t>Output 1</t>
+  </si>
+  <si>
+    <t>Output 2</t>
+  </si>
+  <si>
+    <t>Output 1 = Output 2</t>
   </si>
 </sst>
 </file>
@@ -261,15 +291,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:colOff>752475</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>551846</xdr:colOff>
+      <xdr:colOff>513746</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>28362</xdr:rowOff>
+      <xdr:rowOff>66462</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -292,7 +322,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="790575" y="2133600"/>
+          <a:off x="752475" y="2171700"/>
           <a:ext cx="4828571" cy="1704762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -993,10 +1023,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1299,7 +1325,7 @@
   <dimension ref="A5:AB25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:H27"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02DFE9F-AB1F-473F-8E7C-3831E301DE5F}">
   <dimension ref="A4:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
@@ -1538,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2BC6CF-4EA5-45AC-9B83-7ACDBE94EDCB}">
-  <dimension ref="A4:L4"/>
+  <dimension ref="A4:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,6 +1586,11 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1568,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28208875-80A9-4B1B-923A-4DB12741CFFF}">
-  <dimension ref="A4:P20"/>
+  <dimension ref="A4:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="Q13" sqref="Q13:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1610,7 @@
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1594,7 +1625,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1602,7 +1633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1615,9 +1646,17 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>47</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="13:13" x14ac:dyDescent="0.25">
@@ -1633,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308A7ACF-7C8B-4410-A5E7-DF76C94601A2}">
-  <dimension ref="A2:Y21"/>
+  <dimension ref="A2:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,12 +1731,12 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1707,6 +1746,35 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R24" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1717,7 +1785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F711AFD-61B5-4942-87CF-4165CC64815B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
State Balancing - First workflows
</commit_message>
<xml_diff>
--- a/Documentation/Lists/Balancing State Locations List.xlsx
+++ b/Documentation/Lists/Balancing State Locations List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{D03E98AE-FEDD-4C8F-96F0-36C099982A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9451FA0A-31A4-4813-B3EA-E27BC01D32D7}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{D03E98AE-FEDD-4C8F-96F0-36C099982A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6E153E-51F5-4110-A82F-11056A1252CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{CCEB6A6A-7B34-4562-B81A-A16DD9604AAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{CCEB6A6A-7B34-4562-B81A-A16DD9604AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="TN" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="OK" sheetId="7" r:id="rId6"/>
     <sheet name="CA" sheetId="8" r:id="rId7"/>
     <sheet name="CO DR-0100 XML" sheetId="9" r:id="rId8"/>
+    <sheet name="SC" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
   <si>
     <t>TN Checkbox Locatiion</t>
   </si>
@@ -225,16 +226,153 @@
   </si>
   <si>
     <t>Output 1 = Output 2</t>
+  </si>
+  <si>
+    <t>Inputs that we need</t>
+  </si>
+  <si>
+    <t>CO DR-0100 XML tool.xlsm</t>
+  </si>
+  <si>
+    <t>XLSM file with macros that will help us to get state balancing</t>
+  </si>
+  <si>
+    <t>Detail worksheet</t>
+  </si>
+  <si>
+    <t>This detail file is downloaded from Taxsolver</t>
+  </si>
+  <si>
+    <t>Step by step</t>
+  </si>
+  <si>
+    <t>Go to the detail tab</t>
+  </si>
+  <si>
+    <t>Go to DR 0100 XML form page</t>
+  </si>
+  <si>
+    <t>click on "Export Detail as Worksheet"</t>
+  </si>
+  <si>
+    <t>Save the file in some folder in the P drive</t>
+  </si>
+  <si>
+    <t>This will be just a temp file</t>
+  </si>
+  <si>
+    <t>Copy and paste the Detail worksheet file into the Tool file (in the Detail worksheet)</t>
+  </si>
+  <si>
+    <t>2nd part</t>
+  </si>
+  <si>
+    <t>1st part</t>
+  </si>
+  <si>
+    <t>Go to Information Sheet in Taxsolver</t>
+  </si>
+  <si>
+    <t>Get the State Registration ID</t>
+  </si>
+  <si>
+    <t>State ID</t>
+  </si>
+  <si>
+    <t>Open browser</t>
+  </si>
+  <si>
+    <t>https://www.colorado.gov/revenueonline/</t>
+  </si>
+  <si>
+    <t>Click on Sales and Use Tax --- Find Sales and Use Tax rates</t>
+  </si>
+  <si>
+    <t>At the bottom of the page</t>
+  </si>
+  <si>
+    <t>Click on View Business Location rates</t>
+  </si>
+  <si>
+    <t>Type the State ID (2) into the Colorado Account Number field</t>
+  </si>
+  <si>
+    <t>Wait for the page to load and then, click on Export</t>
+  </si>
+  <si>
+    <t>Download the file</t>
+  </si>
+  <si>
+    <t>Check which browser to use and what configuration each user needs to do before running the bot</t>
+  </si>
+  <si>
+    <t>You can save the file in any location in your local drive</t>
+  </si>
+  <si>
+    <t>The output is a TXT file, which contains the colorado table info</t>
+  </si>
+  <si>
+    <t>Get the text from the TXT file and split by line and by semicolon (;)</t>
+  </si>
+  <si>
+    <t>You must have at the end 19 columns</t>
+  </si>
+  <si>
+    <t>Paste the result datatable into the Tool file, Website worksheet.</t>
+  </si>
+  <si>
+    <t>3hd part - Use XLSM tool file</t>
+  </si>
+  <si>
+    <t>Click on Unhide Columns button</t>
+  </si>
+  <si>
+    <t>Click on Hide Columns button</t>
+  </si>
+  <si>
+    <t>In the Rate-Services Fees worksheet, check if the sum of each column is equals to 0</t>
+  </si>
+  <si>
+    <t>3.1 We can focus on the row 60, which starts with "Level County"</t>
+  </si>
+  <si>
+    <t>3.1 If some of them are different to 0, the bot should mark this as a failure</t>
+  </si>
+  <si>
+    <t>In the Balancing Sheet, check if TAX Not balanced and EXCEPT Not balanced cells are equals to 0</t>
+  </si>
+  <si>
+    <t>4.1 If some of them are different to 0, the bot should mark this as a failure</t>
+  </si>
+  <si>
+    <t>Ask Jay</t>
+  </si>
+  <si>
+    <t>SC ST-389 tool (2).xlsx</t>
+  </si>
+  <si>
+    <t>Go to SC ST 389 form page</t>
+  </si>
+  <si>
+    <t>XLSX file with macros and formulas that will help us to get state balancing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,14 +401,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1397,7 +1538,7 @@
   <dimension ref="A3:Y16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308A7ACF-7C8B-4410-A5E7-DF76C94601A2}">
   <dimension ref="A2:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -1783,14 +1924,372 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F711AFD-61B5-4942-87CF-4165CC64815B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:T1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3.1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3.2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>8.1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>9.1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="M35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G18" r:id="rId1" tooltip="https://www.colorado.gov/revenueonline/" xr:uid="{C9805E69-CCFC-4104-923E-D43E4C3E00D2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2338F6A8-F589-4069-9642-EF8E2E82DFC3}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3.1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3.2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>